<commit_message>
adding info to excell
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\Desktop\descktop 2\last project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\Desktop\abdelhadiLast\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
-    <sheet name="products" sheetId="1" r:id="rId1"/>
+    <sheet name="category" sheetId="1" r:id="rId1"/>
     <sheet name="Books" sheetId="2" r:id="rId2"/>
     <sheet name="logins" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -26,46 +26,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>ProductA</t>
-  </si>
-  <si>
-    <t>ProductC</t>
-  </si>
-  <si>
-    <t>ProductB</t>
-  </si>
-  <si>
     <t>logins</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>3/13/20</t>
-  </si>
-  <si>
-    <t>3/14/20</t>
-  </si>
-  <si>
-    <t>paid</t>
-  </si>
-  <si>
-    <t>quantity</t>
+    <t>Hand Bags</t>
+  </si>
+  <si>
+    <t>Watches</t>
+  </si>
+  <si>
+    <t>Shoes</t>
+  </si>
+  <si>
+    <t>Suits</t>
+  </si>
+  <si>
+    <t>Accessories</t>
+  </si>
+  <si>
+    <t>fragrances</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/8801089/pexels-photo-8801089.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=1</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/190819/pexels-photo-190819.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=1</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/1598505/pexels-photo-1598505.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=1</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/1096849/pexels-photo-1096849.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=1</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/1453008/pexels-photo-1453008.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=1</t>
+  </si>
+  <si>
+    <t>https://images.pexels.com/photos/965989/pexels-photo-965989.jpeg?auto=compress&amp;cs=tinysrgb&amp;w=1260&amp;h=750&amp;dpr=1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,14 +111,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -374,75 +399,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="83.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44166</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>4</v>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -470,7 +505,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>